<commit_message>
Updating examples to show new features
Fix shared charts to use explicit value as expressions will leave values empty.
Add DR chart resize to shared charts.

Show HTML/DOCX embedding in Word.

Add Content Control Dropdown example to XML binding.

DR Chart example added to SheetReport.

Alternative way to present empty table in WordTables
</commit_message>
<xml_diff>
--- a/Advanced/SheetReport/template/Report.xlsx
+++ b/Advanced/SheetReport/template/Report.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Country report" sheetId="5" r:id="rId1"/>
-    <sheet name="{{country.sheetName}}" sheetId="2" r:id="rId2"/>
-    <sheet name="Analysis" sheetId="1" r:id="rId3"/>
-    <sheet name="HiddenData" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="Chart" sheetId="7" r:id="rId2"/>
+    <sheet name="{{country.sheetName}}" sheetId="2" r:id="rId3"/>
+    <sheet name="Analysis" sheetId="1" r:id="rId4"/>
+    <sheet name="HiddenData" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId5"/>
+    <pivotCache cacheId="5" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>City</t>
   </si>
@@ -72,12 +73,18 @@
   <si>
     <t>This pivot table has refresh option enabled which allows it to be displayed properly after Templater changes the data for it.</t>
   </si>
+  <si>
+    <t>{{cities}}</t>
+  </si>
+  <si>
+    <t>{{analysis}}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,20 +142,171 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="hr-HR"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chart!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>{{analysis}}</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Chart!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>{{cities}}</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Chart!$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="493431424"/>
+        <c:axId val="493457792"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="493431424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="493457792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="493457792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="493431424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:view3D>
       <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
       <c:perspective val="30"/>
     </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
     <c:plotArea>
       <c:layout/>
       <c:pie3DChart>
@@ -195,15 +353,23 @@
           </c:val>
         </c:ser>
         <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
           <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
         </c:dLbls>
       </c:pie3DChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -262,6 +428,41 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
       <xdr:row>7</xdr:row>
@@ -294,7 +495,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Author" refreshedDate="43334.977411689812" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Author" refreshedDate="44447.637296527777" createdVersion="3" refreshedVersion="4" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="Table2"/>
   </cacheSource>
@@ -318,6 +519,11 @@
       <sharedItems/>
     </cacheField>
   </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
 </pivotCacheDefinition>
 </file>
 
@@ -333,7 +539,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B4:D8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -391,9 +597,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B8:C9" totalsRowShown="0">
-  <autoFilter ref="B8:C9">
-    <filterColumn colId="1"/>
-  </autoFilter>
+  <autoFilter ref="B8:C9"/>
   <tableColumns count="2">
     <tableColumn id="1" name="City"/>
     <tableColumn id="2" name="Population" dataDxfId="0"/>
@@ -404,9 +608,7 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D2" totalsRowShown="0">
-  <autoFilter ref="A1:D2">
-    <filterColumn colId="1"/>
-  </autoFilter>
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Country"/>
     <tableColumn id="4" name="City"/>
@@ -492,6 +694,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -526,6 +729,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -701,14 +905,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -716,30 +920,60 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="311.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="18.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="23.25">
+    <row r="2" spans="2:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -747,7 +981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -765,15 +999,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
@@ -781,12 +1015,12 @@
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
@@ -794,7 +1028,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -805,7 +1039,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -816,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -827,7 +1061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
@@ -847,22 +1081,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -876,7 +1110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -890,10 +1124,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G6" s="1"/>
     </row>
   </sheetData>

</xml_diff>